<commit_message>
hopefully fixed emoji problem
</commit_message>
<xml_diff>
--- a/0_literature/list-sources.xlsx
+++ b/0_literature/list-sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\consulting\projects\consulting\2_code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\consulting\projects\consulting\0_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7039B8-1470-4E8B-BCC1-3468ACC3DCEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6FCA19-A9AE-457F-9564-F0559E0D6995}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4A97FC25-B009-4150-BADE-91670A5B071B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A97FC25-B009-4150-BADE-91670A5B071B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>type</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>https://www.clarin.si/repository/xmlui/handle/11356/1048</t>
+  </si>
+  <si>
+    <t>emojis_unicode</t>
+  </si>
+  <si>
+    <t>https://github.com/today-is-a-good-day/emojis/blob/master/emDict.csv</t>
   </si>
 </sst>
 </file>
@@ -474,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34BDCA7-D9EE-4F93-8502-106E608DCE56}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,6 +581,15 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>